<commit_message>
Added readme and updated docs
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCT-7269-02\Documents\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pete Canfield\Desktop\4320_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38046518-0720-4E4E-AFAC-AA3C1CC125E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-23190" yWindow="-120" windowWidth="23310" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,9 +51,6 @@
     <t>Mark as issue</t>
   </si>
   <si>
-    <t>Any use logged in can mark an issue in the project.</t>
-  </si>
-  <si>
     <t>Contributor</t>
   </si>
   <si>
@@ -78,12 +76,15 @@
   </si>
   <si>
     <t>System sorts contributors based on issue worked on within project.</t>
+  </si>
+  <si>
+    <t>Any user logged in can mark an issue in the project.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -461,11 +462,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
@@ -501,35 +502,35 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
@@ -540,10 +541,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
@@ -554,10 +555,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -645,7 +646,7 @@
       <c r="D20" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D20">
     <sortCondition ref="B2:B20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>